<commit_message>
firstly useful while recommend notebooks
</commit_message>
<xml_diff>
--- a/sources/laptops.xlsx
+++ b/sources/laptops.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fowillwly/Dev/shopping_bot/sources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F30B855-EF2A-3144-AE77-99BB216C73D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCB987C2-F47D-FD4E-90C5-DADF7F911192}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="26380" windowHeight="15540" xr2:uid="{61AB98E8-4DBE-F945-961E-200BFA28F3C5}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="50">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -205,6 +205,27 @@
   <si>
     <t>screen-r1</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>big-screen</t>
+  </si>
+  <si>
+    <t>small-screen</t>
+  </si>
+  <si>
+    <t>too-heavy</t>
+  </si>
+  <si>
+    <t>high-performance</t>
+  </si>
+  <si>
+    <t>low-performance</t>
+  </si>
+  <si>
+    <t>too-expensive</t>
+  </si>
+  <si>
+    <t>to-cheap</t>
   </si>
 </sst>
 </file>
@@ -571,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE7FF8E4-0800-4641-925F-239C11CA1B8C}">
-  <dimension ref="A1:X6"/>
+  <dimension ref="A1:AE6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+    <sheetView tabSelected="1" topLeftCell="X1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="AE14" sqref="AE14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -590,10 +611,14 @@
     <col min="22" max="22" width="16.5" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:31">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -666,8 +691,29 @@
       <c r="X1" t="s">
         <v>17</v>
       </c>
+      <c r="Y1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>49</v>
+      </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:31">
       <c r="A2">
         <v>1</v>
       </c>
@@ -740,8 +786,29 @@
       <c r="X2">
         <v>6</v>
       </c>
+      <c r="Y2">
+        <v>9</v>
+      </c>
+      <c r="Z2">
+        <v>5</v>
+      </c>
+      <c r="AA2">
+        <v>6</v>
+      </c>
+      <c r="AB2">
+        <v>7.5</v>
+      </c>
+      <c r="AC2">
+        <v>6.5</v>
+      </c>
+      <c r="AD2">
+        <v>3</v>
+      </c>
+      <c r="AE2">
+        <v>9</v>
+      </c>
     </row>
-    <row r="3" spans="1:24">
+    <row r="3" spans="1:31">
       <c r="A3">
         <v>2</v>
       </c>
@@ -814,8 +881,29 @@
       <c r="X3">
         <v>7</v>
       </c>
+      <c r="Y3">
+        <v>8</v>
+      </c>
+      <c r="Z3">
+        <v>6</v>
+      </c>
+      <c r="AA3">
+        <v>7</v>
+      </c>
+      <c r="AB3">
+        <v>7</v>
+      </c>
+      <c r="AC3">
+        <v>7</v>
+      </c>
+      <c r="AD3">
+        <v>4</v>
+      </c>
+      <c r="AE3">
+        <v>8</v>
+      </c>
     </row>
-    <row r="4" spans="1:24">
+    <row r="4" spans="1:31">
       <c r="A4">
         <v>3</v>
       </c>
@@ -888,8 +976,29 @@
       <c r="X4">
         <v>6</v>
       </c>
+      <c r="Y4">
+        <v>6</v>
+      </c>
+      <c r="Z4">
+        <v>7</v>
+      </c>
+      <c r="AA4">
+        <v>8</v>
+      </c>
+      <c r="AB4">
+        <v>6.5</v>
+      </c>
+      <c r="AC4">
+        <v>7.5</v>
+      </c>
+      <c r="AD4">
+        <v>6</v>
+      </c>
+      <c r="AE4">
+        <v>6</v>
+      </c>
     </row>
-    <row r="5" spans="1:24">
+    <row r="5" spans="1:31">
       <c r="A5">
         <v>4</v>
       </c>
@@ -962,8 +1071,29 @@
       <c r="X5">
         <v>6</v>
       </c>
+      <c r="Y5">
+        <v>5</v>
+      </c>
+      <c r="Z5">
+        <v>8</v>
+      </c>
+      <c r="AA5">
+        <v>7.5</v>
+      </c>
+      <c r="AB5">
+        <v>6</v>
+      </c>
+      <c r="AC5">
+        <v>8</v>
+      </c>
+      <c r="AD5">
+        <v>8</v>
+      </c>
+      <c r="AE5">
+        <v>4</v>
+      </c>
     </row>
-    <row r="6" spans="1:24">
+    <row r="6" spans="1:31">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1035,6 +1165,27 @@
       </c>
       <c r="X6">
         <v>8</v>
+      </c>
+      <c r="Y6">
+        <v>8</v>
+      </c>
+      <c r="Z6">
+        <v>6</v>
+      </c>
+      <c r="AA6">
+        <v>3</v>
+      </c>
+      <c r="AB6">
+        <v>9</v>
+      </c>
+      <c r="AC6">
+        <v>5</v>
+      </c>
+      <c r="AD6">
+        <v>7</v>
+      </c>
+      <c r="AE6">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>